<commit_message>
replaced csv with Xlsx
</commit_message>
<xml_diff>
--- a/reports/test_report.xlsx
+++ b/reports/test_report.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="currency_filtering_test" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="currency_filtering_test1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -618,4 +619,205 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>page_url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>testcase</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>passed</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Currency Change to US</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De $767', 'De $719', 'De $1,168', 'De $161', 'De $366', 'De $117', 'De $741', 'De $496', 'De $722', 'De $269', 'De $1,995', 'De $69', 'De $1,448', 'De $215', 'De $1,071', 'De $539', 'De $591', 'De $234', 'De $1,089', 'De $111', 'De $121', 'De $227', 'De $380', 'De $524']</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Currency Change to CA</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De $1,079', 'De $1,012', 'De $1,643', 'De $226', 'De $515', 'De $165', 'De $1,043', 'De $698', 'De $1,016', 'De $378', 'De $2,807', 'De $96', 'De $2,037', 'De $302', 'De $1,507', 'De $758', 'De $832', 'De $329', 'De $1,532', 'De $156', 'De $170', 'De $320', 'De $535', 'De $737']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Currency Change to BE</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De €731', 'De €685', 'De €1,113', 'De €153', 'De €349', 'De €112', 'De €706', 'De €473', 'De €688', 'De €256', 'De €1,901', 'De €65', 'De €1,380', 'De €205', 'De €1,021', 'De €514', 'De €563', 'De €223', 'De €1,038', 'De €106', 'De €115', 'De €217', 'De €362', 'De €499']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Currency Change to IE</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De £605', 'De £567', 'De £921', 'De £127', 'De £289', 'De £93', 'De £585', 'De £391', 'De £570', 'De £212', 'De £1,574', 'De £54', 'De £1,142', 'De £170', 'De £845', 'De £425', 'De £467', 'De £184', 'De £859', 'De £88', 'De £95', 'De £179', 'De £300', 'De £413']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Currency Change to AU</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De $1,196', 'De $1,122', 'De $1,822', 'De $251', 'De $571', 'De $183', 'De $1,156', 'De $774', 'De $1,126', 'De $419', 'De $3,111', 'De $107', 'De $2,258', 'De $335', 'De $1,670', 'De $841', 'De $922', 'De $365', 'De $1,698', 'De $173', 'De $189', 'De $355', 'De $593', 'De $817']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Currency Change to SG</t>
+        </is>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De $1,033', 'De $968', 'De $1,573', 'De $217', 'De $493', 'De $158', 'De $998', 'De $668', 'De $972', 'De $362', 'De $2,686', 'De $92', 'De $1,950', 'De $289', 'De $1,442', 'De $726', 'De $796', 'De $315', 'De $1,466', 'De $149', 'De $163', 'De $306', 'De $512', 'De $706']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Currency Change to AE</t>
+        </is>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De د.إ.2,817', 'De د.إ.2,642', 'De د.إ.4,290', 'De د.إ.591', 'De د.إ.1,344', 'De د.إ.431', 'De د.إ.2,722', 'De د.إ.1,822', 'De د.إ.2,652', 'De د.إ.988', 'De د.إ.7,328', 'De د.إ.252', 'De د.إ.5,319', 'De د.إ.790', 'De د.إ.3,934', 'De د.إ.1,980', 'De د.إ.2,172', 'De د.إ.858', 'De د.إ.4,000', 'De د.إ.408', 'De د.إ.444', 'De د.إ.835', 'De د.إ.1,396', 'De د.إ.1,925']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io/property/bonita-casa-de-campo-t%c3%adpica-mallorquina/BC-12224317</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Currency Change to BD</t>
+        </is>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Updated prices: ['De ৳91,716', 'De ৳86,000', 'De ৳139,666', 'De ৳19,241', 'De ৳43,765', 'De ৳14,038', 'De ৳88,607', 'De ৳59,331', 'De ৳86,335', 'De ৳32,160', 'De ৳238,557', 'De ৳8,197', 'De ৳173,148', 'De ৳25,709', 'De ৳128,067', 'De ৳64,452', 'De ৳70,706', 'De ৳27,946', 'De ৳130,220', 'De ৳13,273', 'De ৳14,459', 'De ৳27,186', 'De ৳45,439', 'De ৳62,671']</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>